<commit_message>
add generate support to year 2024
</commit_message>
<xml_diff>
--- a/Data2024.xlsx
+++ b/Data2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7994c8fb138f2f6/Documents/CU_Year3/projects/ShiftWorkScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4745177D-F362-4B72-8B5D-A72FD6A2A640}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB4C7D5-7263-411A-8F32-56847E32D7CD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
change schedule algorithm due to requirement
</commit_message>
<xml_diff>
--- a/Data2024.xlsx
+++ b/Data2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7994c8fb138f2f6/Documents/CU_Year3/projects/ShiftWorkScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB4C7D5-7263-411A-8F32-56847E32D7CD}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95AB6C40-CEE6-4496-854F-4B1B856AEEEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36340" yWindow="-4670" windowWidth="34680" windowHeight="19020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -735,14 +735,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="67.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
     <col min="6" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="9" width="27.42578125" customWidth="1"/>
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>

</xml_diff>